<commit_message>
0814 Mitra Store OTW
</commit_message>
<xml_diff>
--- a/Dokumen/Halaman Web.xlsx
+++ b/Dokumen/Halaman Web.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Pro\DepositoSyariah\Dev\MainDepositoSyariah\dokumen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C774BF18-FE46-4C1C-9B8F-7B45C34D5665}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E0AD661-DF9A-44BA-A204-55A6CA529A2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,10 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -162,7 +159,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -178,6 +175,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -248,7 +251,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -262,9 +265,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -274,6 +274,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -591,10 +598,10 @@
   <dimension ref="B2:BK58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="5" ySplit="4" topLeftCell="F8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="4" topLeftCell="F11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomRight" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,75 +609,75 @@
     <col min="1" max="1" width="2.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="5.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="19.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="2"/>
     <col min="6" max="63" width="3" style="1" customWidth="1"/>
     <col min="64" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
-      <c r="U2" s="7"/>
-      <c r="V2" s="7"/>
-      <c r="W2" s="7"/>
-      <c r="X2" s="7"/>
-      <c r="Y2" s="7"/>
-      <c r="Z2" s="7"/>
-      <c r="AA2" s="7"/>
-      <c r="AB2" s="7"/>
-      <c r="AC2" s="7"/>
-      <c r="AD2" s="7"/>
-      <c r="AE2" s="7"/>
-      <c r="AF2" s="7"/>
-      <c r="AG2" s="7"/>
-      <c r="AH2" s="7" t="s">
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
+      <c r="U2" s="10"/>
+      <c r="V2" s="10"/>
+      <c r="W2" s="10"/>
+      <c r="X2" s="10"/>
+      <c r="Y2" s="10"/>
+      <c r="Z2" s="10"/>
+      <c r="AA2" s="10"/>
+      <c r="AB2" s="10"/>
+      <c r="AC2" s="10"/>
+      <c r="AD2" s="10"/>
+      <c r="AE2" s="10"/>
+      <c r="AF2" s="10"/>
+      <c r="AG2" s="10"/>
+      <c r="AH2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="AI2" s="7"/>
-      <c r="AJ2" s="7"/>
-      <c r="AK2" s="7"/>
-      <c r="AL2" s="7"/>
-      <c r="AM2" s="7"/>
-      <c r="AN2" s="7"/>
-      <c r="AO2" s="7"/>
-      <c r="AP2" s="7"/>
-      <c r="AQ2" s="7"/>
-      <c r="AR2" s="7"/>
-      <c r="AS2" s="7"/>
-      <c r="AT2" s="7"/>
-      <c r="AU2" s="7"/>
-      <c r="AV2" s="7"/>
-      <c r="AW2" s="7"/>
-      <c r="AX2" s="7"/>
-      <c r="AY2" s="7"/>
-      <c r="AZ2" s="7"/>
-      <c r="BA2" s="7"/>
-      <c r="BB2" s="7"/>
-      <c r="BC2" s="7"/>
-      <c r="BD2" s="7"/>
-      <c r="BE2" s="7"/>
-      <c r="BF2" s="7"/>
-      <c r="BG2" s="7"/>
-      <c r="BH2" s="7"/>
-      <c r="BI2" s="7"/>
-      <c r="BJ2" s="7"/>
-      <c r="BK2" s="7"/>
+      <c r="AI2" s="10"/>
+      <c r="AJ2" s="10"/>
+      <c r="AK2" s="10"/>
+      <c r="AL2" s="10"/>
+      <c r="AM2" s="10"/>
+      <c r="AN2" s="10"/>
+      <c r="AO2" s="10"/>
+      <c r="AP2" s="10"/>
+      <c r="AQ2" s="10"/>
+      <c r="AR2" s="10"/>
+      <c r="AS2" s="10"/>
+      <c r="AT2" s="10"/>
+      <c r="AU2" s="10"/>
+      <c r="AV2" s="10"/>
+      <c r="AW2" s="10"/>
+      <c r="AX2" s="10"/>
+      <c r="AY2" s="10"/>
+      <c r="AZ2" s="10"/>
+      <c r="BA2" s="10"/>
+      <c r="BB2" s="10"/>
+      <c r="BC2" s="10"/>
+      <c r="BD2" s="10"/>
+      <c r="BE2" s="10"/>
+      <c r="BF2" s="10"/>
+      <c r="BG2" s="10"/>
+      <c r="BH2" s="10"/>
+      <c r="BI2" s="10"/>
+      <c r="BJ2" s="10"/>
+      <c r="BK2" s="10"/>
     </row>
     <row r="3" spans="2:63" x14ac:dyDescent="0.25">
       <c r="F3" s="4">
@@ -849,7 +856,7 @@
       </c>
     </row>
     <row r="4" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B4" s="8">
+      <c r="B4" s="7">
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -1035,7 +1042,7 @@
       </c>
     </row>
     <row r="5" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B5" s="9"/>
+      <c r="B5" s="8"/>
       <c r="C5" s="4">
         <v>1</v>
       </c>
@@ -1103,7 +1110,7 @@
       <c r="BK5" s="3"/>
     </row>
     <row r="6" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B6" s="9"/>
+      <c r="B6" s="8"/>
       <c r="C6" s="4">
         <v>2</v>
       </c>
@@ -1171,7 +1178,7 @@
       <c r="BK6" s="3"/>
     </row>
     <row r="7" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B7" s="9"/>
+      <c r="B7" s="8"/>
       <c r="C7" s="4">
         <v>3</v>
       </c>
@@ -1239,7 +1246,7 @@
       <c r="BK7" s="3"/>
     </row>
     <row r="8" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B8" s="9"/>
+      <c r="B8" s="8"/>
       <c r="C8" s="4">
         <v>4</v>
       </c>
@@ -1307,7 +1314,7 @@
       <c r="BK8" s="3"/>
     </row>
     <row r="9" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B9" s="9"/>
+      <c r="B9" s="8"/>
       <c r="C9" s="4">
         <v>5</v>
       </c>
@@ -1375,7 +1382,7 @@
       <c r="BK9" s="3"/>
     </row>
     <row r="10" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B10" s="10"/>
+      <c r="B10" s="9"/>
       <c r="C10" s="4">
         <v>6</v>
       </c>
@@ -1443,7 +1450,7 @@
       <c r="BK10" s="3"/>
     </row>
     <row r="11" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B11" s="8">
+      <c r="B11" s="7">
         <v>2</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -1511,7 +1518,7 @@
       <c r="BK11" s="3"/>
     </row>
     <row r="12" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B12" s="9"/>
+      <c r="B12" s="8"/>
       <c r="C12" s="4">
         <v>1</v>
       </c>
@@ -1581,7 +1588,7 @@
       <c r="BK12" s="3"/>
     </row>
     <row r="13" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B13" s="9"/>
+      <c r="B13" s="8"/>
       <c r="C13" s="4">
         <v>2</v>
       </c>
@@ -1649,7 +1656,7 @@
       <c r="BK13" s="3"/>
     </row>
     <row r="14" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B14" s="9"/>
+      <c r="B14" s="8"/>
       <c r="C14" s="4">
         <v>3</v>
       </c>
@@ -1717,11 +1724,11 @@
       <c r="BK14" s="3"/>
     </row>
     <row r="15" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B15" s="9"/>
+      <c r="B15" s="8"/>
       <c r="C15" s="4">
         <v>4</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="12" t="s">
         <v>11</v>
       </c>
       <c r="E15" s="4"/>
@@ -1785,14 +1792,16 @@
       <c r="BK15" s="3"/>
     </row>
     <row r="16" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B16" s="9"/>
+      <c r="B16" s="8"/>
       <c r="C16" s="4">
         <v>5</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="4"/>
+      <c r="E16" s="4">
+        <v>100</v>
+      </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
@@ -1853,7 +1862,7 @@
       <c r="BK16" s="3"/>
     </row>
     <row r="17" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B17" s="9"/>
+      <c r="B17" s="8"/>
       <c r="C17" s="4">
         <v>6</v>
       </c>
@@ -1921,7 +1930,7 @@
       <c r="BK17" s="3"/>
     </row>
     <row r="18" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B18" s="9"/>
+      <c r="B18" s="8"/>
       <c r="C18" s="4">
         <v>7</v>
       </c>
@@ -1989,7 +1998,7 @@
       <c r="BK18" s="3"/>
     </row>
     <row r="19" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B19" s="9"/>
+      <c r="B19" s="8"/>
       <c r="C19" s="4">
         <v>8</v>
       </c>
@@ -2057,7 +2066,7 @@
       <c r="BK19" s="3"/>
     </row>
     <row r="20" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B20" s="9"/>
+      <c r="B20" s="8"/>
       <c r="C20" s="4">
         <v>9</v>
       </c>
@@ -2125,7 +2134,7 @@
       <c r="BK20" s="3"/>
     </row>
     <row r="21" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B21" s="9"/>
+      <c r="B21" s="8"/>
       <c r="C21" s="4">
         <v>10</v>
       </c>
@@ -2193,11 +2202,11 @@
       <c r="BK21" s="3"/>
     </row>
     <row r="22" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B22" s="9"/>
+      <c r="B22" s="8"/>
       <c r="C22" s="4">
         <v>11</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="12" t="s">
         <v>16</v>
       </c>
       <c r="E22" s="4"/>
@@ -2261,7 +2270,7 @@
       <c r="BK22" s="3"/>
     </row>
     <row r="23" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B23" s="9"/>
+      <c r="B23" s="8"/>
       <c r="C23" s="4">
         <v>12</v>
       </c>
@@ -2329,11 +2338,11 @@
       <c r="BK23" s="3"/>
     </row>
     <row r="24" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B24" s="10"/>
+      <c r="B24" s="9"/>
       <c r="C24" s="4">
         <v>13</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="12" t="s">
         <v>18</v>
       </c>
       <c r="E24" s="4"/>
@@ -2397,7 +2406,7 @@
       <c r="BK24" s="3"/>
     </row>
     <row r="25" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B25" s="8">
+      <c r="B25" s="7">
         <v>3</v>
       </c>
       <c r="C25" s="3" t="s">
@@ -2465,7 +2474,7 @@
       <c r="BK25" s="3"/>
     </row>
     <row r="26" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B26" s="9"/>
+      <c r="B26" s="8"/>
       <c r="C26" s="4">
         <v>1</v>
       </c>
@@ -2535,7 +2544,7 @@
       <c r="BK26" s="3"/>
     </row>
     <row r="27" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B27" s="9"/>
+      <c r="B27" s="8"/>
       <c r="C27" s="4">
         <v>2</v>
       </c>
@@ -2603,7 +2612,7 @@
       <c r="BK27" s="3"/>
     </row>
     <row r="28" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B28" s="9"/>
+      <c r="B28" s="8"/>
       <c r="C28" s="4">
         <v>3</v>
       </c>
@@ -2671,7 +2680,7 @@
       <c r="BK28" s="3"/>
     </row>
     <row r="29" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B29" s="9"/>
+      <c r="B29" s="8"/>
       <c r="C29" s="4">
         <v>4</v>
       </c>
@@ -2739,7 +2748,7 @@
       <c r="BK29" s="3"/>
     </row>
     <row r="30" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B30" s="9"/>
+      <c r="B30" s="8"/>
       <c r="C30" s="4">
         <v>5</v>
       </c>
@@ -2807,7 +2816,7 @@
       <c r="BK30" s="3"/>
     </row>
     <row r="31" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B31" s="9"/>
+      <c r="B31" s="8"/>
       <c r="C31" s="4">
         <v>6</v>
       </c>
@@ -2875,7 +2884,7 @@
       <c r="BK31" s="3"/>
     </row>
     <row r="32" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B32" s="9"/>
+      <c r="B32" s="8"/>
       <c r="C32" s="4">
         <v>7</v>
       </c>
@@ -2943,7 +2952,7 @@
       <c r="BK32" s="3"/>
     </row>
     <row r="33" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B33" s="9"/>
+      <c r="B33" s="8"/>
       <c r="C33" s="4">
         <v>8</v>
       </c>
@@ -3011,7 +3020,7 @@
       <c r="BK33" s="3"/>
     </row>
     <row r="34" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B34" s="9"/>
+      <c r="B34" s="8"/>
       <c r="C34" s="4">
         <v>9</v>
       </c>
@@ -3079,7 +3088,7 @@
       <c r="BK34" s="3"/>
     </row>
     <row r="35" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B35" s="9"/>
+      <c r="B35" s="8"/>
       <c r="C35" s="4">
         <v>10</v>
       </c>
@@ -3147,7 +3156,7 @@
       <c r="BK35" s="3"/>
     </row>
     <row r="36" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B36" s="10"/>
+      <c r="B36" s="9"/>
       <c r="C36" s="4">
         <v>11</v>
       </c>
@@ -3215,7 +3224,7 @@
       <c r="BK36" s="3"/>
     </row>
     <row r="37" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B37" s="8">
+      <c r="B37" s="7">
         <v>4</v>
       </c>
       <c r="C37" s="3" t="s">
@@ -3283,7 +3292,7 @@
       <c r="BK37" s="3"/>
     </row>
     <row r="38" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B38" s="9"/>
+      <c r="B38" s="8"/>
       <c r="C38" s="4">
         <v>1</v>
       </c>
@@ -3353,7 +3362,7 @@
       <c r="BK38" s="3"/>
     </row>
     <row r="39" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B39" s="9"/>
+      <c r="B39" s="8"/>
       <c r="C39" s="4">
         <v>2</v>
       </c>
@@ -3361,7 +3370,7 @@
         <v>9</v>
       </c>
       <c r="E39" s="4">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
@@ -3423,7 +3432,7 @@
       <c r="BK39" s="3"/>
     </row>
     <row r="40" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B40" s="9"/>
+      <c r="B40" s="8"/>
       <c r="C40" s="4">
         <v>3</v>
       </c>
@@ -3493,14 +3502,16 @@
       <c r="BK40" s="3"/>
     </row>
     <row r="41" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B41" s="9"/>
+      <c r="B41" s="8"/>
       <c r="C41" s="4">
         <v>4</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E41" s="4"/>
+      <c r="E41" s="4">
+        <v>90</v>
+      </c>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
@@ -3561,7 +3572,7 @@
       <c r="BK41" s="3"/>
     </row>
     <row r="42" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B42" s="9"/>
+      <c r="B42" s="8"/>
       <c r="C42" s="4">
         <v>5</v>
       </c>
@@ -3569,7 +3580,7 @@
         <v>13</v>
       </c>
       <c r="E42" s="4">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
@@ -3631,16 +3642,14 @@
       <c r="BK42" s="3"/>
     </row>
     <row r="43" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B43" s="9"/>
+      <c r="B43" s="8"/>
       <c r="C43" s="4">
         <v>6</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E43" s="4">
-        <v>70</v>
-      </c>
+      <c r="E43" s="4"/>
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
       <c r="H43" s="5"/>
@@ -3701,7 +3710,7 @@
       <c r="BK43" s="3"/>
     </row>
     <row r="44" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B44" s="9"/>
+      <c r="B44" s="8"/>
       <c r="C44" s="4">
         <v>7</v>
       </c>
@@ -3709,7 +3718,7 @@
         <v>14</v>
       </c>
       <c r="E44" s="4">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
@@ -3771,11 +3780,11 @@
       <c r="BK44" s="3"/>
     </row>
     <row r="45" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B45" s="9"/>
-      <c r="C45" s="4">
+      <c r="B45" s="8"/>
+      <c r="C45" s="11">
         <v>8</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D45" s="12" t="s">
         <v>4</v>
       </c>
       <c r="E45" s="4"/>
@@ -3839,11 +3848,11 @@
       <c r="BK45" s="3"/>
     </row>
     <row r="46" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B46" s="9"/>
-      <c r="C46" s="4">
+      <c r="B46" s="8"/>
+      <c r="C46" s="11">
         <v>9</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="D46" s="12" t="s">
         <v>18</v>
       </c>
       <c r="E46" s="4"/>
@@ -3907,7 +3916,7 @@
       <c r="BK46" s="3"/>
     </row>
     <row r="47" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B47" s="10"/>
+      <c r="B47" s="9"/>
       <c r="C47" s="4">
         <v>10</v>
       </c>
@@ -3975,7 +3984,7 @@
       <c r="BK47" s="3"/>
     </row>
     <row r="48" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B48" s="8">
+      <c r="B48" s="7">
         <v>5</v>
       </c>
       <c r="C48" s="3" t="s">
@@ -4043,7 +4052,7 @@
       <c r="BK48" s="3"/>
     </row>
     <row r="49" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B49" s="9"/>
+      <c r="B49" s="8"/>
       <c r="C49" s="4">
         <v>1</v>
       </c>
@@ -4113,7 +4122,7 @@
       <c r="BK49" s="3"/>
     </row>
     <row r="50" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B50" s="9"/>
+      <c r="B50" s="8"/>
       <c r="C50" s="4">
         <v>2</v>
       </c>
@@ -4181,7 +4190,7 @@
       <c r="BK50" s="3"/>
     </row>
     <row r="51" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B51" s="9"/>
+      <c r="B51" s="8"/>
       <c r="C51" s="4">
         <v>3</v>
       </c>
@@ -4249,7 +4258,7 @@
       <c r="BK51" s="3"/>
     </row>
     <row r="52" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B52" s="9"/>
+      <c r="B52" s="8"/>
       <c r="C52" s="4">
         <v>4</v>
       </c>
@@ -4317,7 +4326,7 @@
       <c r="BK52" s="3"/>
     </row>
     <row r="53" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B53" s="9"/>
+      <c r="B53" s="8"/>
       <c r="C53" s="4">
         <v>5</v>
       </c>
@@ -4385,7 +4394,7 @@
       <c r="BK53" s="3"/>
     </row>
     <row r="54" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B54" s="9"/>
+      <c r="B54" s="8"/>
       <c r="C54" s="4">
         <v>6</v>
       </c>
@@ -4453,7 +4462,7 @@
       <c r="BK54" s="3"/>
     </row>
     <row r="55" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B55" s="9"/>
+      <c r="B55" s="8"/>
       <c r="C55" s="4">
         <v>7</v>
       </c>
@@ -4521,7 +4530,7 @@
       <c r="BK55" s="3"/>
     </row>
     <row r="56" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B56" s="9"/>
+      <c r="B56" s="8"/>
       <c r="C56" s="4">
         <v>8</v>
       </c>
@@ -4589,7 +4598,7 @@
       <c r="BK56" s="3"/>
     </row>
     <row r="57" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B57" s="10"/>
+      <c r="B57" s="9"/>
       <c r="C57" s="4">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
0815 Fixing Mitra Nasabah
</commit_message>
<xml_diff>
--- a/Dokumen/Halaman Web.xlsx
+++ b/Dokumen/Halaman Web.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Pro\DepositoSyariah\Dev\MainDepositoSyariah\dokumen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E0AD661-DF9A-44BA-A204-55A6CA529A2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8BD8284-8064-42FA-8BE0-AF273615733E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -265,6 +265,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -277,10 +281,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -598,10 +598,10 @@
   <dimension ref="B2:BK58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="5" ySplit="4" topLeftCell="F11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="4" topLeftCell="F14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="D16" sqref="D16"/>
+      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,68 +616,68 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
-      <c r="T2" s="10"/>
-      <c r="U2" s="10"/>
-      <c r="V2" s="10"/>
-      <c r="W2" s="10"/>
-      <c r="X2" s="10"/>
-      <c r="Y2" s="10"/>
-      <c r="Z2" s="10"/>
-      <c r="AA2" s="10"/>
-      <c r="AB2" s="10"/>
-      <c r="AC2" s="10"/>
-      <c r="AD2" s="10"/>
-      <c r="AE2" s="10"/>
-      <c r="AF2" s="10"/>
-      <c r="AG2" s="10"/>
-      <c r="AH2" s="10" t="s">
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12"/>
+      <c r="S2" s="12"/>
+      <c r="T2" s="12"/>
+      <c r="U2" s="12"/>
+      <c r="V2" s="12"/>
+      <c r="W2" s="12"/>
+      <c r="X2" s="12"/>
+      <c r="Y2" s="12"/>
+      <c r="Z2" s="12"/>
+      <c r="AA2" s="12"/>
+      <c r="AB2" s="12"/>
+      <c r="AC2" s="12"/>
+      <c r="AD2" s="12"/>
+      <c r="AE2" s="12"/>
+      <c r="AF2" s="12"/>
+      <c r="AG2" s="12"/>
+      <c r="AH2" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="AI2" s="10"/>
-      <c r="AJ2" s="10"/>
-      <c r="AK2" s="10"/>
-      <c r="AL2" s="10"/>
-      <c r="AM2" s="10"/>
-      <c r="AN2" s="10"/>
-      <c r="AO2" s="10"/>
-      <c r="AP2" s="10"/>
-      <c r="AQ2" s="10"/>
-      <c r="AR2" s="10"/>
-      <c r="AS2" s="10"/>
-      <c r="AT2" s="10"/>
-      <c r="AU2" s="10"/>
-      <c r="AV2" s="10"/>
-      <c r="AW2" s="10"/>
-      <c r="AX2" s="10"/>
-      <c r="AY2" s="10"/>
-      <c r="AZ2" s="10"/>
-      <c r="BA2" s="10"/>
-      <c r="BB2" s="10"/>
-      <c r="BC2" s="10"/>
-      <c r="BD2" s="10"/>
-      <c r="BE2" s="10"/>
-      <c r="BF2" s="10"/>
-      <c r="BG2" s="10"/>
-      <c r="BH2" s="10"/>
-      <c r="BI2" s="10"/>
-      <c r="BJ2" s="10"/>
-      <c r="BK2" s="10"/>
+      <c r="AI2" s="12"/>
+      <c r="AJ2" s="12"/>
+      <c r="AK2" s="12"/>
+      <c r="AL2" s="12"/>
+      <c r="AM2" s="12"/>
+      <c r="AN2" s="12"/>
+      <c r="AO2" s="12"/>
+      <c r="AP2" s="12"/>
+      <c r="AQ2" s="12"/>
+      <c r="AR2" s="12"/>
+      <c r="AS2" s="12"/>
+      <c r="AT2" s="12"/>
+      <c r="AU2" s="12"/>
+      <c r="AV2" s="12"/>
+      <c r="AW2" s="12"/>
+      <c r="AX2" s="12"/>
+      <c r="AY2" s="12"/>
+      <c r="AZ2" s="12"/>
+      <c r="BA2" s="12"/>
+      <c r="BB2" s="12"/>
+      <c r="BC2" s="12"/>
+      <c r="BD2" s="12"/>
+      <c r="BE2" s="12"/>
+      <c r="BF2" s="12"/>
+      <c r="BG2" s="12"/>
+      <c r="BH2" s="12"/>
+      <c r="BI2" s="12"/>
+      <c r="BJ2" s="12"/>
+      <c r="BK2" s="12"/>
     </row>
     <row r="3" spans="2:63" x14ac:dyDescent="0.25">
       <c r="F3" s="4">
@@ -856,7 +856,7 @@
       </c>
     </row>
     <row r="4" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B4" s="7">
+      <c r="B4" s="9">
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -1042,7 +1042,7 @@
       </c>
     </row>
     <row r="5" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B5" s="8"/>
+      <c r="B5" s="10"/>
       <c r="C5" s="4">
         <v>1</v>
       </c>
@@ -1110,7 +1110,7 @@
       <c r="BK5" s="3"/>
     </row>
     <row r="6" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B6" s="8"/>
+      <c r="B6" s="10"/>
       <c r="C6" s="4">
         <v>2</v>
       </c>
@@ -1178,7 +1178,7 @@
       <c r="BK6" s="3"/>
     </row>
     <row r="7" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B7" s="8"/>
+      <c r="B7" s="10"/>
       <c r="C7" s="4">
         <v>3</v>
       </c>
@@ -1246,7 +1246,7 @@
       <c r="BK7" s="3"/>
     </row>
     <row r="8" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B8" s="8"/>
+      <c r="B8" s="10"/>
       <c r="C8" s="4">
         <v>4</v>
       </c>
@@ -1314,7 +1314,7 @@
       <c r="BK8" s="3"/>
     </row>
     <row r="9" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B9" s="8"/>
+      <c r="B9" s="10"/>
       <c r="C9" s="4">
         <v>5</v>
       </c>
@@ -1382,7 +1382,7 @@
       <c r="BK9" s="3"/>
     </row>
     <row r="10" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B10" s="9"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="4">
         <v>6</v>
       </c>
@@ -1450,7 +1450,7 @@
       <c r="BK10" s="3"/>
     </row>
     <row r="11" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B11" s="7">
+      <c r="B11" s="9">
         <v>2</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -1518,7 +1518,7 @@
       <c r="BK11" s="3"/>
     </row>
     <row r="12" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B12" s="8"/>
+      <c r="B12" s="10"/>
       <c r="C12" s="4">
         <v>1</v>
       </c>
@@ -1588,7 +1588,7 @@
       <c r="BK12" s="3"/>
     </row>
     <row r="13" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B13" s="8"/>
+      <c r="B13" s="10"/>
       <c r="C13" s="4">
         <v>2</v>
       </c>
@@ -1656,7 +1656,7 @@
       <c r="BK13" s="3"/>
     </row>
     <row r="14" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B14" s="8"/>
+      <c r="B14" s="10"/>
       <c r="C14" s="4">
         <v>3</v>
       </c>
@@ -1724,14 +1724,16 @@
       <c r="BK14" s="3"/>
     </row>
     <row r="15" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B15" s="8"/>
+      <c r="B15" s="10"/>
       <c r="C15" s="4">
         <v>4</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="4"/>
+      <c r="E15" s="4">
+        <v>50</v>
+      </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
@@ -1792,7 +1794,7 @@
       <c r="BK15" s="3"/>
     </row>
     <row r="16" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B16" s="8"/>
+      <c r="B16" s="10"/>
       <c r="C16" s="4">
         <v>5</v>
       </c>
@@ -1862,7 +1864,7 @@
       <c r="BK16" s="3"/>
     </row>
     <row r="17" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B17" s="8"/>
+      <c r="B17" s="10"/>
       <c r="C17" s="4">
         <v>6</v>
       </c>
@@ -1930,7 +1932,7 @@
       <c r="BK17" s="3"/>
     </row>
     <row r="18" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B18" s="8"/>
+      <c r="B18" s="10"/>
       <c r="C18" s="4">
         <v>7</v>
       </c>
@@ -1998,14 +2000,14 @@
       <c r="BK18" s="3"/>
     </row>
     <row r="19" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B19" s="8"/>
+      <c r="B19" s="10"/>
       <c r="C19" s="4">
         <v>8</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="4"/>
+      <c r="E19" s="7"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
@@ -2066,14 +2068,14 @@
       <c r="BK19" s="3"/>
     </row>
     <row r="20" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B20" s="8"/>
+      <c r="B20" s="10"/>
       <c r="C20" s="4">
         <v>9</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E20" s="4"/>
+      <c r="E20" s="7"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
@@ -2134,14 +2136,14 @@
       <c r="BK20" s="3"/>
     </row>
     <row r="21" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B21" s="8"/>
+      <c r="B21" s="10"/>
       <c r="C21" s="4">
         <v>10</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E21" s="4"/>
+      <c r="E21" s="7"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
@@ -2202,14 +2204,14 @@
       <c r="BK21" s="3"/>
     </row>
     <row r="22" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B22" s="8"/>
+      <c r="B22" s="10"/>
       <c r="C22" s="4">
         <v>11</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D22" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E22" s="4"/>
+      <c r="E22" s="7"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
@@ -2270,7 +2272,7 @@
       <c r="BK22" s="3"/>
     </row>
     <row r="23" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B23" s="8"/>
+      <c r="B23" s="10"/>
       <c r="C23" s="4">
         <v>12</v>
       </c>
@@ -2338,14 +2340,14 @@
       <c r="BK23" s="3"/>
     </row>
     <row r="24" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B24" s="9"/>
+      <c r="B24" s="11"/>
       <c r="C24" s="4">
         <v>13</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="D24" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E24" s="4"/>
+      <c r="E24" s="7"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
@@ -2406,7 +2408,7 @@
       <c r="BK24" s="3"/>
     </row>
     <row r="25" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B25" s="7">
+      <c r="B25" s="9">
         <v>3</v>
       </c>
       <c r="C25" s="3" t="s">
@@ -2474,7 +2476,7 @@
       <c r="BK25" s="3"/>
     </row>
     <row r="26" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B26" s="8"/>
+      <c r="B26" s="10"/>
       <c r="C26" s="4">
         <v>1</v>
       </c>
@@ -2544,7 +2546,7 @@
       <c r="BK26" s="3"/>
     </row>
     <row r="27" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B27" s="8"/>
+      <c r="B27" s="10"/>
       <c r="C27" s="4">
         <v>2</v>
       </c>
@@ -2612,7 +2614,7 @@
       <c r="BK27" s="3"/>
     </row>
     <row r="28" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B28" s="8"/>
+      <c r="B28" s="10"/>
       <c r="C28" s="4">
         <v>3</v>
       </c>
@@ -2680,7 +2682,7 @@
       <c r="BK28" s="3"/>
     </row>
     <row r="29" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B29" s="8"/>
+      <c r="B29" s="10"/>
       <c r="C29" s="4">
         <v>4</v>
       </c>
@@ -2748,7 +2750,7 @@
       <c r="BK29" s="3"/>
     </row>
     <row r="30" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B30" s="8"/>
+      <c r="B30" s="10"/>
       <c r="C30" s="4">
         <v>5</v>
       </c>
@@ -2816,7 +2818,7 @@
       <c r="BK30" s="3"/>
     </row>
     <row r="31" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B31" s="8"/>
+      <c r="B31" s="10"/>
       <c r="C31" s="4">
         <v>6</v>
       </c>
@@ -2884,7 +2886,7 @@
       <c r="BK31" s="3"/>
     </row>
     <row r="32" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B32" s="8"/>
+      <c r="B32" s="10"/>
       <c r="C32" s="4">
         <v>7</v>
       </c>
@@ -2952,7 +2954,7 @@
       <c r="BK32" s="3"/>
     </row>
     <row r="33" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B33" s="8"/>
+      <c r="B33" s="10"/>
       <c r="C33" s="4">
         <v>8</v>
       </c>
@@ -3020,7 +3022,7 @@
       <c r="BK33" s="3"/>
     </row>
     <row r="34" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B34" s="8"/>
+      <c r="B34" s="10"/>
       <c r="C34" s="4">
         <v>9</v>
       </c>
@@ -3088,7 +3090,7 @@
       <c r="BK34" s="3"/>
     </row>
     <row r="35" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B35" s="8"/>
+      <c r="B35" s="10"/>
       <c r="C35" s="4">
         <v>10</v>
       </c>
@@ -3156,7 +3158,7 @@
       <c r="BK35" s="3"/>
     </row>
     <row r="36" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B36" s="9"/>
+      <c r="B36" s="11"/>
       <c r="C36" s="4">
         <v>11</v>
       </c>
@@ -3224,7 +3226,7 @@
       <c r="BK36" s="3"/>
     </row>
     <row r="37" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B37" s="7">
+      <c r="B37" s="9">
         <v>4</v>
       </c>
       <c r="C37" s="3" t="s">
@@ -3292,7 +3294,7 @@
       <c r="BK37" s="3"/>
     </row>
     <row r="38" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B38" s="8"/>
+      <c r="B38" s="10"/>
       <c r="C38" s="4">
         <v>1</v>
       </c>
@@ -3362,7 +3364,7 @@
       <c r="BK38" s="3"/>
     </row>
     <row r="39" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B39" s="8"/>
+      <c r="B39" s="10"/>
       <c r="C39" s="4">
         <v>2</v>
       </c>
@@ -3432,14 +3434,14 @@
       <c r="BK39" s="3"/>
     </row>
     <row r="40" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B40" s="8"/>
-      <c r="C40" s="4">
+      <c r="B40" s="10"/>
+      <c r="C40" s="7">
         <v>3</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D40" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E40" s="4">
+      <c r="E40" s="7">
         <v>100</v>
       </c>
       <c r="F40" s="3"/>
@@ -3502,15 +3504,15 @@
       <c r="BK40" s="3"/>
     </row>
     <row r="41" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B41" s="8"/>
-      <c r="C41" s="4">
+      <c r="B41" s="10"/>
+      <c r="C41" s="7">
         <v>4</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="D41" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E41" s="4">
-        <v>90</v>
+      <c r="E41" s="7">
+        <v>100</v>
       </c>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
@@ -3572,15 +3574,15 @@
       <c r="BK41" s="3"/>
     </row>
     <row r="42" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B42" s="8"/>
-      <c r="C42" s="4">
+      <c r="B42" s="10"/>
+      <c r="C42" s="7">
         <v>5</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D42" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E42" s="4">
-        <v>80</v>
+      <c r="E42" s="7">
+        <v>100</v>
       </c>
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
@@ -3642,7 +3644,7 @@
       <c r="BK42" s="3"/>
     </row>
     <row r="43" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B43" s="8"/>
+      <c r="B43" s="10"/>
       <c r="C43" s="4">
         <v>6</v>
       </c>
@@ -3710,15 +3712,15 @@
       <c r="BK43" s="3"/>
     </row>
     <row r="44" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B44" s="8"/>
-      <c r="C44" s="4">
+      <c r="B44" s="10"/>
+      <c r="C44" s="7">
         <v>7</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D44" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E44" s="4">
-        <v>90</v>
+      <c r="E44" s="7">
+        <v>100</v>
       </c>
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
@@ -3780,14 +3782,14 @@
       <c r="BK44" s="3"/>
     </row>
     <row r="45" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B45" s="8"/>
-      <c r="C45" s="11">
+      <c r="B45" s="10"/>
+      <c r="C45" s="7">
         <v>8</v>
       </c>
-      <c r="D45" s="12" t="s">
+      <c r="D45" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E45" s="4"/>
+      <c r="E45" s="7"/>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
@@ -3848,14 +3850,14 @@
       <c r="BK45" s="3"/>
     </row>
     <row r="46" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B46" s="8"/>
-      <c r="C46" s="11">
+      <c r="B46" s="10"/>
+      <c r="C46" s="7">
         <v>9</v>
       </c>
-      <c r="D46" s="12" t="s">
+      <c r="D46" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E46" s="4"/>
+      <c r="E46" s="7"/>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
@@ -3916,7 +3918,7 @@
       <c r="BK46" s="3"/>
     </row>
     <row r="47" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B47" s="9"/>
+      <c r="B47" s="11"/>
       <c r="C47" s="4">
         <v>10</v>
       </c>
@@ -3984,7 +3986,7 @@
       <c r="BK47" s="3"/>
     </row>
     <row r="48" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B48" s="7">
+      <c r="B48" s="9">
         <v>5</v>
       </c>
       <c r="C48" s="3" t="s">
@@ -4052,7 +4054,7 @@
       <c r="BK48" s="3"/>
     </row>
     <row r="49" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B49" s="8"/>
+      <c r="B49" s="10"/>
       <c r="C49" s="4">
         <v>1</v>
       </c>
@@ -4122,7 +4124,7 @@
       <c r="BK49" s="3"/>
     </row>
     <row r="50" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B50" s="8"/>
+      <c r="B50" s="10"/>
       <c r="C50" s="4">
         <v>2</v>
       </c>
@@ -4190,7 +4192,7 @@
       <c r="BK50" s="3"/>
     </row>
     <row r="51" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B51" s="8"/>
+      <c r="B51" s="10"/>
       <c r="C51" s="4">
         <v>3</v>
       </c>
@@ -4258,7 +4260,7 @@
       <c r="BK51" s="3"/>
     </row>
     <row r="52" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B52" s="8"/>
+      <c r="B52" s="10"/>
       <c r="C52" s="4">
         <v>4</v>
       </c>
@@ -4326,7 +4328,7 @@
       <c r="BK52" s="3"/>
     </row>
     <row r="53" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B53" s="8"/>
+      <c r="B53" s="10"/>
       <c r="C53" s="4">
         <v>5</v>
       </c>
@@ -4394,7 +4396,7 @@
       <c r="BK53" s="3"/>
     </row>
     <row r="54" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B54" s="8"/>
+      <c r="B54" s="10"/>
       <c r="C54" s="4">
         <v>6</v>
       </c>
@@ -4462,7 +4464,7 @@
       <c r="BK54" s="3"/>
     </row>
     <row r="55" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B55" s="8"/>
+      <c r="B55" s="10"/>
       <c r="C55" s="4">
         <v>7</v>
       </c>
@@ -4530,7 +4532,7 @@
       <c r="BK55" s="3"/>
     </row>
     <row r="56" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B56" s="8"/>
+      <c r="B56" s="10"/>
       <c r="C56" s="4">
         <v>8</v>
       </c>
@@ -4598,7 +4600,7 @@
       <c r="BK56" s="3"/>
     </row>
     <row r="57" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B57" s="9"/>
+      <c r="B57" s="11"/>
       <c r="C57" s="4">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
0815 Add Rek Bank Modal
</commit_message>
<xml_diff>
--- a/Dokumen/Halaman Web.xlsx
+++ b/Dokumen/Halaman Web.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Pro\DepositoSyariah\Dev\MainDepositoSyariah\dokumen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8BD8284-8064-42FA-8BE0-AF273615733E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C9214AE-D9E3-4106-B23D-F6E55181551F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -598,10 +598,10 @@
   <dimension ref="B2:BK58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="5" ySplit="4" topLeftCell="F14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="4" topLeftCell="F32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
+      <selection pane="bottomRight" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1732,7 +1732,7 @@
         <v>11</v>
       </c>
       <c r="E15" s="4">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
@@ -2143,7 +2143,9 @@
       <c r="D21" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E21" s="7"/>
+      <c r="E21" s="7">
+        <v>10</v>
+      </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
@@ -3789,7 +3791,9 @@
       <c r="D45" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E45" s="7"/>
+      <c r="E45" s="7">
+        <v>100</v>
+      </c>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
@@ -3857,7 +3861,9 @@
       <c r="D46" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E46" s="7"/>
+      <c r="E46" s="7">
+        <v>100</v>
+      </c>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>

</xml_diff>

<commit_message>
0816 User Akses Done
</commit_message>
<xml_diff>
--- a/Dokumen/Halaman Web.xlsx
+++ b/Dokumen/Halaman Web.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Pro\DepositoSyariah\Dev\MainDepositoSyariah\dokumen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C9214AE-D9E3-4106-B23D-F6E55181551F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3347BF8B-4E06-40E8-9CAF-9A7F97945269}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -598,10 +598,10 @@
   <dimension ref="B2:BK58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="5" ySplit="4" topLeftCell="F32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="4" topLeftCell="F26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E21" sqref="E21"/>
+      <selection pane="bottomRight" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1868,10 +1868,10 @@
       <c r="C17" s="4">
         <v>6</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E17" s="4"/>
+      <c r="E17" s="7"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
@@ -1936,10 +1936,10 @@
       <c r="C18" s="4">
         <v>7</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="4"/>
+      <c r="E18" s="7"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>

</xml_diff>

<commit_message>
0818 Finish UI 85%
</commit_message>
<xml_diff>
--- a/Dokumen/Halaman Web.xlsx
+++ b/Dokumen/Halaman Web.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Pro\DepositoSyariah\Dev\MainDepositoSyariah\dokumen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3347BF8B-4E06-40E8-9CAF-9A7F97945269}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B58966F-B459-46A9-A807-3DD56B9C34AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -598,10 +598,10 @@
   <dimension ref="B2:BK58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="5" ySplit="4" topLeftCell="F26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="4" topLeftCell="F11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E17" sqref="E17"/>
+      <selection pane="bottomRight" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1871,7 +1871,9 @@
       <c r="D17" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E17" s="7"/>
+      <c r="E17" s="7">
+        <v>100</v>
+      </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
@@ -1939,7 +1941,9 @@
       <c r="D18" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="7"/>
+      <c r="E18" s="7">
+        <v>100</v>
+      </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
@@ -2005,9 +2009,11 @@
         <v>8</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" s="7"/>
+        <v>14</v>
+      </c>
+      <c r="E19" s="7">
+        <v>100</v>
+      </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
@@ -2075,7 +2081,9 @@
       <c r="D20" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E20" s="7"/>
+      <c r="E20" s="7">
+        <v>100</v>
+      </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
@@ -2144,7 +2152,7 @@
         <v>15</v>
       </c>
       <c r="E21" s="7">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
@@ -2213,7 +2221,9 @@
       <c r="D22" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E22" s="7"/>
+      <c r="E22" s="7">
+        <v>100</v>
+      </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
@@ -2349,7 +2359,9 @@
       <c r="D24" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E24" s="7"/>
+      <c r="E24" s="7">
+        <v>100</v>
+      </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>

</xml_diff>

<commit_message>
0821 Update Profil Header
</commit_message>
<xml_diff>
--- a/Dokumen/Halaman Web.xlsx
+++ b/Dokumen/Halaman Web.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Pro\DepositoSyariah\Dev\MainDepositoSyariah\dokumen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B58966F-B459-46A9-A807-3DD56B9C34AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE4C2959-F7C5-4685-9ADF-4BB6AECD1572}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -93,9 +93,6 @@
     <t>Web Admin Mitra BPR</t>
   </si>
   <si>
-    <t>Halaman Transaksi</t>
-  </si>
-  <si>
     <t>Web Nasabah</t>
   </si>
   <si>
@@ -142,6 +139,9 @@
   </si>
   <si>
     <t>K</t>
+  </si>
+  <si>
+    <t>Halaman Detail Portofolio</t>
   </si>
 </sst>
 </file>
@@ -251,7 +251,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -279,6 +279,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -598,10 +601,10 @@
   <dimension ref="B2:BK58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="5" ySplit="4" topLeftCell="F11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="4" topLeftCell="F35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E25" sqref="E25"/>
+      <selection pane="bottomRight" activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,7 +620,7 @@
   <sheetData>
     <row r="2" spans="2:63" x14ac:dyDescent="0.25">
       <c r="F2" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -647,7 +650,7 @@
       <c r="AF2" s="12"/>
       <c r="AG2" s="12"/>
       <c r="AH2" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AI2" s="12"/>
       <c r="AJ2" s="12"/>
@@ -864,181 +867,181 @@
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="I4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="L4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="O4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="P4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="V4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="W4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="X4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z4" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="L4" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="M4" s="4" t="s">
+      <c r="AA4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB4" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="AC4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="AD4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF4" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="P4" s="4" t="s">
+      <c r="AG4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="AH4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="AK4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AL4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AM4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="AO4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AP4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AQ4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="R4" s="4" t="s">
+      <c r="AR4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AS4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AU4" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="S4" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="T4" s="4" t="s">
+      <c r="AV4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AW4" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="U4" s="4" t="s">
+      <c r="AX4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="V4" s="4" t="s">
+      <c r="AY4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AZ4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="BA4" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="W4" s="4" t="s">
+      <c r="BB4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="BC4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="BD4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="BE4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="X4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y4" s="4" t="s">
+      <c r="BF4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="BG4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="BH4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="BI4" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="Z4" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA4" s="4" t="s">
+      <c r="BJ4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="BK4" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="AB4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AC4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AD4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AE4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AF4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="AG4" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH4" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AJ4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AK4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AL4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AM4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="AN4" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="AO4" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="AP4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AQ4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AR4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AS4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AT4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="AU4" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="AV4" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="AW4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AX4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AY4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AZ4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="BA4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="BB4" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="BC4" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="BD4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="BE4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="BF4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="BG4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="BH4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="BI4" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="BJ4" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="BK4" s="4" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="5" spans="2:63" x14ac:dyDescent="0.25">
@@ -1592,10 +1595,10 @@
       <c r="C13" s="4">
         <v>2</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="4"/>
+      <c r="E13" s="7"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -1660,10 +1663,10 @@
       <c r="C14" s="4">
         <v>3</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="4"/>
+      <c r="E14" s="7"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -2079,7 +2082,7 @@
         <v>9</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E20" s="7">
         <v>100</v>
@@ -2564,10 +2567,10 @@
       <c r="C27" s="4">
         <v>2</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E27" s="4"/>
+      <c r="E27" s="7"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
@@ -2632,10 +2635,10 @@
       <c r="C28" s="4">
         <v>3</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E28" s="4"/>
+      <c r="E28" s="7"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
@@ -2700,10 +2703,10 @@
       <c r="C29" s="4">
         <v>4</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E29" s="4"/>
+      <c r="E29" s="7"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
@@ -2768,10 +2771,10 @@
       <c r="C30" s="4">
         <v>5</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E30" s="4"/>
+      <c r="E30" s="7"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
@@ -2836,10 +2839,10 @@
       <c r="C31" s="4">
         <v>6</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E31" s="4"/>
+      <c r="E31" s="7"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
@@ -2904,10 +2907,10 @@
       <c r="C32" s="4">
         <v>7</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E32" s="4"/>
+      <c r="E32" s="7"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
@@ -3244,7 +3247,7 @@
         <v>4</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="4"/>
@@ -3309,13 +3312,13 @@
     </row>
     <row r="38" spans="2:63" x14ac:dyDescent="0.25">
       <c r="B38" s="10"/>
-      <c r="C38" s="4">
+      <c r="C38" s="13">
         <v>1</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D38" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E38" s="4">
+      <c r="E38" s="13">
         <v>100</v>
       </c>
       <c r="F38" s="3"/>
@@ -3379,13 +3382,13 @@
     </row>
     <row r="39" spans="2:63" x14ac:dyDescent="0.25">
       <c r="B39" s="10"/>
-      <c r="C39" s="4">
+      <c r="C39" s="13">
         <v>2</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D39" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E39" s="4">
+      <c r="E39" s="13">
         <v>100</v>
       </c>
       <c r="F39" s="5"/>
@@ -3663,7 +3666,7 @@
         <v>6</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="5"/>
@@ -4008,7 +4011,7 @@
         <v>5</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D48" s="3"/>
       <c r="E48" s="4"/>
@@ -4283,7 +4286,7 @@
         <v>4</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E52" s="4"/>
       <c r="F52" s="3"/>
@@ -4351,7 +4354,7 @@
         <v>5</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E53" s="4"/>
       <c r="F53" s="3"/>
@@ -4419,7 +4422,7 @@
         <v>6</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E54" s="4"/>
       <c r="F54" s="3"/>
@@ -4623,7 +4626,7 @@
         <v>9</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E57" s="4"/>
       <c r="F57" s="3"/>
@@ -4687,7 +4690,7 @@
     </row>
     <row r="58" spans="2:63" x14ac:dyDescent="0.25">
       <c r="B58" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C58" s="4">
         <f>COUNT(C5:C10,C12:C24,C26:C36,C38:C47,C49:C57)</f>

</xml_diff>

<commit_message>
0822 Admin Produk Fix
</commit_message>
<xml_diff>
--- a/Dokumen/Halaman Web.xlsx
+++ b/Dokumen/Halaman Web.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Pro\DepositoSyariah\Dev\MainDepositoSyariah\dokumen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE4C2959-F7C5-4685-9ADF-4BB6AECD1572}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E9DF59B-E126-4CBE-A620-D5309A3B6F5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -269,6 +269,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -279,9 +282,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -601,10 +601,10 @@
   <dimension ref="B2:BK58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="5" ySplit="4" topLeftCell="F35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="4" topLeftCell="F20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="G49" sqref="G49"/>
+      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,68 +619,68 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
-      <c r="S2" s="12"/>
-      <c r="T2" s="12"/>
-      <c r="U2" s="12"/>
-      <c r="V2" s="12"/>
-      <c r="W2" s="12"/>
-      <c r="X2" s="12"/>
-      <c r="Y2" s="12"/>
-      <c r="Z2" s="12"/>
-      <c r="AA2" s="12"/>
-      <c r="AB2" s="12"/>
-      <c r="AC2" s="12"/>
-      <c r="AD2" s="12"/>
-      <c r="AE2" s="12"/>
-      <c r="AF2" s="12"/>
-      <c r="AG2" s="12"/>
-      <c r="AH2" s="12" t="s">
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
+      <c r="S2" s="13"/>
+      <c r="T2" s="13"/>
+      <c r="U2" s="13"/>
+      <c r="V2" s="13"/>
+      <c r="W2" s="13"/>
+      <c r="X2" s="13"/>
+      <c r="Y2" s="13"/>
+      <c r="Z2" s="13"/>
+      <c r="AA2" s="13"/>
+      <c r="AB2" s="13"/>
+      <c r="AC2" s="13"/>
+      <c r="AD2" s="13"/>
+      <c r="AE2" s="13"/>
+      <c r="AF2" s="13"/>
+      <c r="AG2" s="13"/>
+      <c r="AH2" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="AI2" s="12"/>
-      <c r="AJ2" s="12"/>
-      <c r="AK2" s="12"/>
-      <c r="AL2" s="12"/>
-      <c r="AM2" s="12"/>
-      <c r="AN2" s="12"/>
-      <c r="AO2" s="12"/>
-      <c r="AP2" s="12"/>
-      <c r="AQ2" s="12"/>
-      <c r="AR2" s="12"/>
-      <c r="AS2" s="12"/>
-      <c r="AT2" s="12"/>
-      <c r="AU2" s="12"/>
-      <c r="AV2" s="12"/>
-      <c r="AW2" s="12"/>
-      <c r="AX2" s="12"/>
-      <c r="AY2" s="12"/>
-      <c r="AZ2" s="12"/>
-      <c r="BA2" s="12"/>
-      <c r="BB2" s="12"/>
-      <c r="BC2" s="12"/>
-      <c r="BD2" s="12"/>
-      <c r="BE2" s="12"/>
-      <c r="BF2" s="12"/>
-      <c r="BG2" s="12"/>
-      <c r="BH2" s="12"/>
-      <c r="BI2" s="12"/>
-      <c r="BJ2" s="12"/>
-      <c r="BK2" s="12"/>
+      <c r="AI2" s="13"/>
+      <c r="AJ2" s="13"/>
+      <c r="AK2" s="13"/>
+      <c r="AL2" s="13"/>
+      <c r="AM2" s="13"/>
+      <c r="AN2" s="13"/>
+      <c r="AO2" s="13"/>
+      <c r="AP2" s="13"/>
+      <c r="AQ2" s="13"/>
+      <c r="AR2" s="13"/>
+      <c r="AS2" s="13"/>
+      <c r="AT2" s="13"/>
+      <c r="AU2" s="13"/>
+      <c r="AV2" s="13"/>
+      <c r="AW2" s="13"/>
+      <c r="AX2" s="13"/>
+      <c r="AY2" s="13"/>
+      <c r="AZ2" s="13"/>
+      <c r="BA2" s="13"/>
+      <c r="BB2" s="13"/>
+      <c r="BC2" s="13"/>
+      <c r="BD2" s="13"/>
+      <c r="BE2" s="13"/>
+      <c r="BF2" s="13"/>
+      <c r="BG2" s="13"/>
+      <c r="BH2" s="13"/>
+      <c r="BI2" s="13"/>
+      <c r="BJ2" s="13"/>
+      <c r="BK2" s="13"/>
     </row>
     <row r="3" spans="2:63" x14ac:dyDescent="0.25">
       <c r="F3" s="4">
@@ -859,7 +859,7 @@
       </c>
     </row>
     <row r="4" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B4" s="9">
+      <c r="B4" s="10">
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -1045,7 +1045,7 @@
       </c>
     </row>
     <row r="5" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B5" s="10"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="4">
         <v>1</v>
       </c>
@@ -1113,7 +1113,7 @@
       <c r="BK5" s="3"/>
     </row>
     <row r="6" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B6" s="10"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="4">
         <v>2</v>
       </c>
@@ -1181,7 +1181,7 @@
       <c r="BK6" s="3"/>
     </row>
     <row r="7" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B7" s="10"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="4">
         <v>3</v>
       </c>
@@ -1249,7 +1249,7 @@
       <c r="BK7" s="3"/>
     </row>
     <row r="8" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B8" s="10"/>
+      <c r="B8" s="11"/>
       <c r="C8" s="4">
         <v>4</v>
       </c>
@@ -1317,7 +1317,7 @@
       <c r="BK8" s="3"/>
     </row>
     <row r="9" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B9" s="10"/>
+      <c r="B9" s="11"/>
       <c r="C9" s="4">
         <v>5</v>
       </c>
@@ -1385,7 +1385,7 @@
       <c r="BK9" s="3"/>
     </row>
     <row r="10" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B10" s="11"/>
+      <c r="B10" s="12"/>
       <c r="C10" s="4">
         <v>6</v>
       </c>
@@ -1453,7 +1453,7 @@
       <c r="BK10" s="3"/>
     </row>
     <row r="11" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B11" s="9">
+      <c r="B11" s="10">
         <v>2</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -1521,7 +1521,7 @@
       <c r="BK11" s="3"/>
     </row>
     <row r="12" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B12" s="10"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="4">
         <v>1</v>
       </c>
@@ -1591,14 +1591,16 @@
       <c r="BK12" s="3"/>
     </row>
     <row r="13" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B13" s="10"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="4">
         <v>2</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="7"/>
+      <c r="E13" s="7">
+        <v>100</v>
+      </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -1659,7 +1661,7 @@
       <c r="BK13" s="3"/>
     </row>
     <row r="14" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B14" s="10"/>
+      <c r="B14" s="11"/>
       <c r="C14" s="4">
         <v>3</v>
       </c>
@@ -1727,7 +1729,7 @@
       <c r="BK14" s="3"/>
     </row>
     <row r="15" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B15" s="10"/>
+      <c r="B15" s="11"/>
       <c r="C15" s="4">
         <v>4</v>
       </c>
@@ -1797,7 +1799,7 @@
       <c r="BK15" s="3"/>
     </row>
     <row r="16" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B16" s="10"/>
+      <c r="B16" s="11"/>
       <c r="C16" s="4">
         <v>5</v>
       </c>
@@ -1867,7 +1869,7 @@
       <c r="BK16" s="3"/>
     </row>
     <row r="17" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B17" s="10"/>
+      <c r="B17" s="11"/>
       <c r="C17" s="4">
         <v>6</v>
       </c>
@@ -1937,7 +1939,7 @@
       <c r="BK17" s="3"/>
     </row>
     <row r="18" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B18" s="10"/>
+      <c r="B18" s="11"/>
       <c r="C18" s="4">
         <v>7</v>
       </c>
@@ -2007,7 +2009,7 @@
       <c r="BK18" s="3"/>
     </row>
     <row r="19" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B19" s="10"/>
+      <c r="B19" s="11"/>
       <c r="C19" s="4">
         <v>8</v>
       </c>
@@ -2077,7 +2079,7 @@
       <c r="BK19" s="3"/>
     </row>
     <row r="20" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B20" s="10"/>
+      <c r="B20" s="11"/>
       <c r="C20" s="4">
         <v>9</v>
       </c>
@@ -2147,7 +2149,7 @@
       <c r="BK20" s="3"/>
     </row>
     <row r="21" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B21" s="10"/>
+      <c r="B21" s="11"/>
       <c r="C21" s="4">
         <v>10</v>
       </c>
@@ -2217,7 +2219,7 @@
       <c r="BK21" s="3"/>
     </row>
     <row r="22" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B22" s="10"/>
+      <c r="B22" s="11"/>
       <c r="C22" s="4">
         <v>11</v>
       </c>
@@ -2287,7 +2289,7 @@
       <c r="BK22" s="3"/>
     </row>
     <row r="23" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B23" s="10"/>
+      <c r="B23" s="11"/>
       <c r="C23" s="4">
         <v>12</v>
       </c>
@@ -2355,7 +2357,7 @@
       <c r="BK23" s="3"/>
     </row>
     <row r="24" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B24" s="11"/>
+      <c r="B24" s="12"/>
       <c r="C24" s="4">
         <v>13</v>
       </c>
@@ -2425,7 +2427,7 @@
       <c r="BK24" s="3"/>
     </row>
     <row r="25" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B25" s="9">
+      <c r="B25" s="10">
         <v>3</v>
       </c>
       <c r="C25" s="3" t="s">
@@ -2493,7 +2495,7 @@
       <c r="BK25" s="3"/>
     </row>
     <row r="26" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B26" s="10"/>
+      <c r="B26" s="11"/>
       <c r="C26" s="4">
         <v>1</v>
       </c>
@@ -2563,14 +2565,16 @@
       <c r="BK26" s="3"/>
     </row>
     <row r="27" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B27" s="10"/>
+      <c r="B27" s="11"/>
       <c r="C27" s="4">
         <v>2</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E27" s="7"/>
+      <c r="E27" s="7">
+        <v>100</v>
+      </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
@@ -2631,7 +2635,7 @@
       <c r="BK27" s="3"/>
     </row>
     <row r="28" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B28" s="10"/>
+      <c r="B28" s="11"/>
       <c r="C28" s="4">
         <v>3</v>
       </c>
@@ -2699,7 +2703,7 @@
       <c r="BK28" s="3"/>
     </row>
     <row r="29" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B29" s="10"/>
+      <c r="B29" s="11"/>
       <c r="C29" s="4">
         <v>4</v>
       </c>
@@ -2767,7 +2771,7 @@
       <c r="BK29" s="3"/>
     </row>
     <row r="30" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B30" s="10"/>
+      <c r="B30" s="11"/>
       <c r="C30" s="4">
         <v>5</v>
       </c>
@@ -2835,7 +2839,7 @@
       <c r="BK30" s="3"/>
     </row>
     <row r="31" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B31" s="10"/>
+      <c r="B31" s="11"/>
       <c r="C31" s="4">
         <v>6</v>
       </c>
@@ -2903,7 +2907,7 @@
       <c r="BK31" s="3"/>
     </row>
     <row r="32" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B32" s="10"/>
+      <c r="B32" s="11"/>
       <c r="C32" s="4">
         <v>7</v>
       </c>
@@ -2971,14 +2975,14 @@
       <c r="BK32" s="3"/>
     </row>
     <row r="33" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B33" s="10"/>
+      <c r="B33" s="11"/>
       <c r="C33" s="4">
         <v>8</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E33" s="4"/>
+      <c r="E33" s="7"/>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
@@ -3039,14 +3043,14 @@
       <c r="BK33" s="3"/>
     </row>
     <row r="34" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B34" s="10"/>
+      <c r="B34" s="11"/>
       <c r="C34" s="4">
         <v>9</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E34" s="4"/>
+      <c r="E34" s="7"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
@@ -3107,14 +3111,14 @@
       <c r="BK34" s="3"/>
     </row>
     <row r="35" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B35" s="10"/>
+      <c r="B35" s="11"/>
       <c r="C35" s="4">
         <v>10</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D35" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E35" s="4"/>
+      <c r="E35" s="7"/>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
@@ -3175,7 +3179,7 @@
       <c r="BK35" s="3"/>
     </row>
     <row r="36" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B36" s="11"/>
+      <c r="B36" s="12"/>
       <c r="C36" s="4">
         <v>11</v>
       </c>
@@ -3243,7 +3247,7 @@
       <c r="BK36" s="3"/>
     </row>
     <row r="37" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B37" s="9">
+      <c r="B37" s="10">
         <v>4</v>
       </c>
       <c r="C37" s="3" t="s">
@@ -3311,14 +3315,14 @@
       <c r="BK37" s="3"/>
     </row>
     <row r="38" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B38" s="10"/>
-      <c r="C38" s="13">
+      <c r="B38" s="11"/>
+      <c r="C38" s="9">
         <v>1</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E38" s="13">
+      <c r="E38" s="9">
         <v>100</v>
       </c>
       <c r="F38" s="3"/>
@@ -3381,14 +3385,14 @@
       <c r="BK38" s="3"/>
     </row>
     <row r="39" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B39" s="10"/>
-      <c r="C39" s="13">
+      <c r="B39" s="11"/>
+      <c r="C39" s="9">
         <v>2</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E39" s="13">
+      <c r="E39" s="9">
         <v>100</v>
       </c>
       <c r="F39" s="5"/>
@@ -3451,7 +3455,7 @@
       <c r="BK39" s="3"/>
     </row>
     <row r="40" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B40" s="10"/>
+      <c r="B40" s="11"/>
       <c r="C40" s="7">
         <v>3</v>
       </c>
@@ -3521,7 +3525,7 @@
       <c r="BK40" s="3"/>
     </row>
     <row r="41" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B41" s="10"/>
+      <c r="B41" s="11"/>
       <c r="C41" s="7">
         <v>4</v>
       </c>
@@ -3591,7 +3595,7 @@
       <c r="BK41" s="3"/>
     </row>
     <row r="42" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B42" s="10"/>
+      <c r="B42" s="11"/>
       <c r="C42" s="7">
         <v>5</v>
       </c>
@@ -3661,7 +3665,7 @@
       <c r="BK42" s="3"/>
     </row>
     <row r="43" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B43" s="10"/>
+      <c r="B43" s="11"/>
       <c r="C43" s="4">
         <v>6</v>
       </c>
@@ -3729,7 +3733,7 @@
       <c r="BK43" s="3"/>
     </row>
     <row r="44" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B44" s="10"/>
+      <c r="B44" s="11"/>
       <c r="C44" s="7">
         <v>7</v>
       </c>
@@ -3799,7 +3803,7 @@
       <c r="BK44" s="3"/>
     </row>
     <row r="45" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B45" s="10"/>
+      <c r="B45" s="11"/>
       <c r="C45" s="7">
         <v>8</v>
       </c>
@@ -3869,7 +3873,7 @@
       <c r="BK45" s="3"/>
     </row>
     <row r="46" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B46" s="10"/>
+      <c r="B46" s="11"/>
       <c r="C46" s="7">
         <v>9</v>
       </c>
@@ -3939,7 +3943,7 @@
       <c r="BK46" s="3"/>
     </row>
     <row r="47" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B47" s="11"/>
+      <c r="B47" s="12"/>
       <c r="C47" s="4">
         <v>10</v>
       </c>
@@ -4007,7 +4011,7 @@
       <c r="BK47" s="3"/>
     </row>
     <row r="48" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B48" s="9">
+      <c r="B48" s="10">
         <v>5</v>
       </c>
       <c r="C48" s="3" t="s">
@@ -4075,7 +4079,7 @@
       <c r="BK48" s="3"/>
     </row>
     <row r="49" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B49" s="10"/>
+      <c r="B49" s="11"/>
       <c r="C49" s="4">
         <v>1</v>
       </c>
@@ -4145,7 +4149,7 @@
       <c r="BK49" s="3"/>
     </row>
     <row r="50" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B50" s="10"/>
+      <c r="B50" s="11"/>
       <c r="C50" s="4">
         <v>2</v>
       </c>
@@ -4213,7 +4217,7 @@
       <c r="BK50" s="3"/>
     </row>
     <row r="51" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B51" s="10"/>
+      <c r="B51" s="11"/>
       <c r="C51" s="4">
         <v>3</v>
       </c>
@@ -4281,7 +4285,7 @@
       <c r="BK51" s="3"/>
     </row>
     <row r="52" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B52" s="10"/>
+      <c r="B52" s="11"/>
       <c r="C52" s="4">
         <v>4</v>
       </c>
@@ -4349,7 +4353,7 @@
       <c r="BK52" s="3"/>
     </row>
     <row r="53" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B53" s="10"/>
+      <c r="B53" s="11"/>
       <c r="C53" s="4">
         <v>5</v>
       </c>
@@ -4417,7 +4421,7 @@
       <c r="BK53" s="3"/>
     </row>
     <row r="54" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B54" s="10"/>
+      <c r="B54" s="11"/>
       <c r="C54" s="4">
         <v>6</v>
       </c>
@@ -4485,7 +4489,7 @@
       <c r="BK54" s="3"/>
     </row>
     <row r="55" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B55" s="10"/>
+      <c r="B55" s="11"/>
       <c r="C55" s="4">
         <v>7</v>
       </c>
@@ -4553,7 +4557,7 @@
       <c r="BK55" s="3"/>
     </row>
     <row r="56" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B56" s="10"/>
+      <c r="B56" s="11"/>
       <c r="C56" s="4">
         <v>8</v>
       </c>
@@ -4621,7 +4625,7 @@
       <c r="BK56" s="3"/>
     </row>
     <row r="57" spans="2:63" x14ac:dyDescent="0.25">
-      <c r="B57" s="11"/>
+      <c r="B57" s="12"/>
       <c r="C57" s="4">
         <v>9</v>
       </c>

</xml_diff>